<commit_message>
Ajout des données xlsx sur le tertiaire
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_tertiaire_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_tertiaire_1D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312DDE04-993D-524F-9591-38D30599260F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD1C3CD-4A4A-0C47-A5F5-4BDD90FF20BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="500" windowWidth="29060" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10040" yWindow="3360" windowWidth="29060" windowHeight="16180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,17 @@
     <sheet name="Energy_source_year" sheetId="4" r:id="rId4"/>
     <sheet name="retrofit_Transition" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -111,7 +121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,12 +140,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -200,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -220,13 +224,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -533,13 +534,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" customWidth="1"/>
@@ -581,7 +582,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B5">
@@ -623,7 +624,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -653,7 +654,7 @@
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -825,10 +826,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B53D8C-8207-B84F-8ED5-7A100CED18F8}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -861,245 +862,13 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="7">
-        <v>2021</v>
+      <c r="A3" s="6">
+        <v>2050</v>
       </c>
       <c r="B3">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="7">
-        <v>2023</v>
-      </c>
-      <c r="B5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="6">
-        <v>2024</v>
-      </c>
-      <c r="B6">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="7">
-        <v>2025</v>
-      </c>
-      <c r="B7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="6">
-        <v>2026</v>
-      </c>
-      <c r="B8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="7">
-        <v>2027</v>
-      </c>
-      <c r="B9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="6">
-        <v>2028</v>
-      </c>
-      <c r="B10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="7">
-        <v>2029</v>
-      </c>
-      <c r="B11">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="6">
-        <v>2030</v>
-      </c>
-      <c r="B12">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="7">
-        <v>2031</v>
-      </c>
-      <c r="B13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="6">
-        <v>2032</v>
-      </c>
-      <c r="B14">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="7">
-        <v>2033</v>
-      </c>
-      <c r="B15">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="6">
-        <v>2034</v>
-      </c>
-      <c r="B16">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="7">
-        <v>2035</v>
-      </c>
-      <c r="B17">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="6">
-        <v>2036</v>
-      </c>
-      <c r="B18">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="7">
-        <v>2037</v>
-      </c>
-      <c r="B19">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="6">
-        <v>2038</v>
-      </c>
-      <c r="B20">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="7">
-        <v>2039</v>
-      </c>
-      <c r="B21">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="6">
-        <v>2040</v>
-      </c>
-      <c r="B22">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="7">
-        <v>2041</v>
-      </c>
-      <c r="B23">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="6">
-        <v>2042</v>
-      </c>
-      <c r="B24">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="7">
-        <v>2043</v>
-      </c>
-      <c r="B25">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="6">
-        <v>2044</v>
-      </c>
-      <c r="B26">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="7">
-        <v>2045</v>
-      </c>
-      <c r="B27">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="6">
-        <v>2046</v>
-      </c>
-      <c r="B28">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="7">
-        <v>2047</v>
-      </c>
-      <c r="B29">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="6">
-        <v>2048</v>
-      </c>
-      <c r="B30">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="7">
-        <v>2049</v>
-      </c>
-      <c r="B31">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="6">
-        <v>2050</v>
-      </c>
-      <c r="B32">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C32">
+      <c r="C3">
         <v>0.3</v>
       </c>
     </row>
@@ -1113,7 +882,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1320,7 +1089,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Ajout du résidentiel 2D et README
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_tertiaire_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_tertiaire_1D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC50B643-8C99-6D4B-A0C9-1E23442AAB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E227BC1-4123-8941-8B17-B99D48B3E327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20780" yWindow="2080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20780" yWindow="2080" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="2" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Valeur</t>
   </si>
   <si>
-    <t>init_Besoin_surfacique</t>
-  </si>
-  <si>
     <t>init_proportion_besoin_chauffage</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Energy_source</t>
   </si>
   <si>
-    <t>init_Surface</t>
-  </si>
-  <si>
     <t>init_conso_unitaire_elec</t>
   </si>
   <si>
@@ -115,6 +109,12 @@
   </si>
   <si>
     <t>new_yearly_repartition_per_Energy_source</t>
+  </si>
+  <si>
+    <t>init_surface</t>
+  </si>
+  <si>
+    <t>init_energy_need_per_surface</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:B3"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -556,7 +556,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>205.31245689655171</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0.65283620689655175</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7523553</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2020</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>2050</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -637,27 +637,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>40726800</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>210049200</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>501552000</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>67748400</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>204120000</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>13996800</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>89326800</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -838,13 +838,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1123,18 +1123,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>2020</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>2020</v>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>2020</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>2020</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>2020</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>2020</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>2020</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>2020</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>2025</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>2025</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>2025</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>2025</v>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>2025</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>2025</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>2025</v>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>2025</v>
@@ -1317,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1337,39 +1337,39 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3">
         <v>2020</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3">
         <v>2020</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3">
         <v>2020</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3">
         <v>2020</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3">
         <v>2020</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3">
         <v>2020</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3">
         <v>2020</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3">
         <v>2020</v>

</xml_diff>

<commit_message>
Ajout de la possibilité d'une date step et détection automatique des dimensions
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_tertiaire_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_tertiaire_1D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{9835FFEC-F744-477B-BEF6-03E50590D26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{544B6AEC-8CE4-4DD0-86B9-789A3DDD3FB3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D376813D-50CE-B247-BE51-80779AF6F181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="2" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -44,9 +42,6 @@
     <t>Valeur</t>
   </si>
   <si>
-    <t>init_Besoin_surfacique</t>
-  </si>
-  <si>
     <t>init_proportion_besoin_chauffage</t>
   </si>
   <si>
@@ -68,9 +63,6 @@
     <t>Energy_source</t>
   </si>
   <si>
-    <t>init_Surface</t>
-  </si>
-  <si>
     <t>init_conso_unitaire_elec</t>
   </si>
   <si>
@@ -120,6 +112,12 @@
   </si>
   <si>
     <t>retrofit_change_surface</t>
+  </si>
+  <si>
+    <t>init_surface</t>
+  </si>
+  <si>
+    <t>init_energy_need_per_surface</t>
   </si>
 </sst>
 </file>
@@ -527,19 +525,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -552,7 +550,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>205.31245689655171</v>
@@ -560,7 +558,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0.65283620689655175</v>
@@ -568,7 +566,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -576,7 +574,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>7523553</v>
@@ -584,7 +582,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2020</v>
@@ -592,7 +590,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>2050</v>
@@ -600,7 +598,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -617,46 +615,46 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>40726800</v>
@@ -679,7 +677,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>210049200</v>
@@ -702,7 +700,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>501552000</v>
@@ -725,7 +723,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>67748400</v>
@@ -748,7 +746,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>204120000</v>
@@ -771,7 +769,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>13996800</v>
@@ -794,7 +792,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>89326800</v>
@@ -817,7 +815,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -848,26 +846,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B53D8C-8207-B84F-8ED5-7A100CED18F8}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -905,27 +903,27 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="45.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>2020</v>
@@ -936,7 +934,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>2020</v>
@@ -947,7 +945,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>2020</v>
@@ -958,7 +956,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>2020</v>
@@ -969,7 +967,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>2020</v>
@@ -980,7 +978,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>2020</v>
@@ -991,7 +989,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>2020</v>
@@ -1002,7 +1000,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>2020</v>
@@ -1013,7 +1011,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>2025</v>
@@ -1024,7 +1022,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>2025</v>
@@ -1035,7 +1033,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>2025</v>
@@ -1046,7 +1044,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>2025</v>
@@ -1057,7 +1055,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>2025</v>
@@ -1068,7 +1066,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>2025</v>
@@ -1079,7 +1077,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>2025</v>
@@ -1090,7 +1088,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>2025</v>
@@ -1112,55 +1110,55 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3">
         <v>2020</v>
@@ -1192,7 +1190,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3">
         <v>2020</v>
@@ -1224,7 +1222,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3">
         <v>2020</v>
@@ -1256,7 +1254,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3">
         <v>2020</v>
@@ -1288,7 +1286,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3">
         <v>2020</v>
@@ -1320,7 +1318,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3">
         <v>2020</v>
@@ -1352,7 +1350,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3">
         <v>2020</v>
@@ -1384,7 +1382,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3">
         <v>2020</v>

</xml_diff>

<commit_message>
suppression de data et Sujets d'analyse
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_tertiaire_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_tertiaire_1D.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A0B1CF-DFCC-0A46-AD2F-4BF572DE8057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC532D2-6EBE-9B43-A8AC-4166370B738B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,7 +526,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>